<commit_message>
refactor: update session details and enhance schedule formatting
</commit_message>
<xml_diff>
--- a/session_schedule_by_slot.xlsx
+++ b/session_schedule_by_slot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjohnson/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AFB405-1621-374D-B680-AB6AA9F4FADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFCA6D4-3EC7-AE4C-9201-41134E039161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>Seyboth: Better Together: How Human Connection Transforms AI into an Effective Educational Partner</t>
   </si>
   <si>
-    <t>Alsamadisi: Alsamadisi (Custom)</t>
-  </si>
-  <si>
     <t>Hojinicki: From Curiosity to Community: Launching a Teacher-Led Gen AI Professional Development Initiative</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>Peterson: Metacognition and AI: Empowering High School Students to Become Strategic Learners in a Technological World</t>
   </si>
   <si>
-    <t>Griggs: Griggs (Custom)</t>
-  </si>
-  <si>
     <t>Scullin: Creating a Student Learning Praxis in the Age of AI</t>
   </si>
   <si>
@@ -142,20 +136,26 @@
     <t>Heckman: Lessons Learned from (Co-Lab)orating Across Schools</t>
   </si>
   <si>
-    <t>MacClintic: Student Presentations (Custom)</t>
-  </si>
-  <si>
-    <t>Chew</t>
-  </si>
-  <si>
-    <t>Nurenberg</t>
+    <t>Chew: Pre-Skilling for the Unknown: Building a Human-Centered AI Culture in Schools</t>
+  </si>
+  <si>
+    <t>Nurenberg: Dangerous (Artificial) Minds: Engaging student critical thinking and analysis in their interactions with AI</t>
+  </si>
+  <si>
+    <t>Alsamadisi: Rethinking Creative and Critical Thinking in the Age of AI</t>
+  </si>
+  <si>
+    <t>Place Based TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MacClintic: Student Presentations </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +182,14 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -233,6 +241,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,7 +553,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -617,11 +626,11 @@
       <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>41</v>
+      <c r="E2" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="3" t="s">
@@ -640,7 +649,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -648,22 +657,22 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>19</v>
@@ -675,13 +684,13 @@
         <v>21</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="109" customHeight="1" x14ac:dyDescent="0.2">
@@ -689,40 +698,40 @@
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="K4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="M4" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance session management for special events and update room assignments
- Updated `sessions.json` to reflect new room assignments and refined tags for various sessions.
- Modified `update_rooms.py` to handle special events (arrival, keynote, closing) by assigning them to a designated location (Hubbard Auditorium).
- Enhanced `update_schedule.py` to create special session objects for events like arrival, keynote, and closing, ensuring they are marked as required for all participants.
</commit_message>
<xml_diff>
--- a/session_schedule_by_slot.xlsx
+++ b/session_schedule_by_slot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjohnson/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFCA6D4-3EC7-AE4C-9201-41134E039161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E93D415-0816-6E43-93E7-E3FD0127C7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15200" yWindow="800" windowWidth="14880" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,43 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
-  <si>
-    <t>Room A</t>
-  </si>
-  <si>
-    <t>Room B</t>
-  </si>
-  <si>
-    <t>Room C</t>
-  </si>
-  <si>
-    <t>Room D</t>
-  </si>
-  <si>
-    <t>Room E</t>
-  </si>
-  <si>
-    <t>Room F</t>
-  </si>
-  <si>
-    <t>Room G</t>
-  </si>
-  <si>
-    <t>Room H</t>
-  </si>
-  <si>
-    <t>Room I</t>
-  </si>
-  <si>
-    <t>Room J</t>
-  </si>
-  <si>
-    <t>Room K</t>
-  </si>
-  <si>
-    <t>Room L</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Time Slot</t>
   </si>
@@ -70,9 +34,6 @@
     <t>Slot 3 (1:30-2:30)</t>
   </si>
   <si>
-    <t>Murphy Paul: Annie Murphy Paul Breakout Session: Deeper Dive into "Thinking with our Surroundings" from The Extended Mind</t>
-  </si>
-  <si>
     <t>Nilsson: What Learning Science Tells Us about Teaching with AI</t>
   </si>
   <si>
@@ -88,9 +49,6 @@
     <t>Lamb: AI-Powered Pedagogy: Crafting Effective Prompts for Transformative Learning</t>
   </si>
   <si>
-    <t>Solomon: Design Thinking Brainstorming (Custom)</t>
-  </si>
-  <si>
     <t>Seyboth: Better Together: How Human Connection Transforms AI into an Effective Educational Partner</t>
   </si>
   <si>
@@ -130,32 +88,89 @@
     <t>Spaletta: AI-Adapted Writing Assignments for Skill Development and AI Literacy</t>
   </si>
   <si>
-    <t>Matlack: Crafting the Future: Customizing Artificial Intelligence (AI) Tools to Enhance Student Experiences &amp; Learning Outcomes in Curriculum Development</t>
-  </si>
-  <si>
     <t>Heckman: Lessons Learned from (Co-Lab)orating Across Schools</t>
   </si>
   <si>
+    <t>Matlack: Place-Based Education in the Era of AI</t>
+  </si>
+  <si>
+    <t>Pearse Hub for Innovation</t>
+  </si>
+  <si>
     <t>Chew: Pre-Skilling for the Unknown: Building a Human-Centered AI Culture in Schools</t>
   </si>
   <si>
-    <t>Nurenberg: Dangerous (Artificial) Minds: Engaging student critical thinking and analysis in their interactions with AI</t>
+    <t>Solomon: Untethered Thinking: Design Thinking Frameworks for Tech-Free Student Brainstorms</t>
+  </si>
+  <si>
+    <t>Hubbard Auditorium</t>
+  </si>
+  <si>
+    <t>Paul: Annie Murphy Paul Breakout Session: Deeper Dive into "Thinking with our Surroundings" from The Extended Mind</t>
   </si>
   <si>
     <t>Alsamadisi: Rethinking Creative and Critical Thinking in the Age of AI</t>
   </si>
   <si>
-    <t>Place Based TBD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MacClintic: Student Presentations </t>
+    <t>MacClintic: Teaching Student Presentation Skills</t>
+  </si>
+  <si>
+    <t>Kravis Center</t>
+  </si>
+  <si>
+    <t>Brush 201</t>
+  </si>
+  <si>
+    <t>Brush 203</t>
+  </si>
+  <si>
+    <t>Brush 202</t>
+  </si>
+  <si>
+    <t>Brush 302</t>
+  </si>
+  <si>
+    <t>Brush 314</t>
+  </si>
+  <si>
+    <t>Writing Center</t>
+  </si>
+  <si>
+    <t>Brush 2nd Floor</t>
+  </si>
+  <si>
+    <t>Brush 310</t>
+  </si>
+  <si>
+    <t>Brush 308</t>
+  </si>
+  <si>
+    <t>Brush 306</t>
+  </si>
+  <si>
+    <t>Welcome &amp; Keynote</t>
+  </si>
+  <si>
+    <t>Closing</t>
+  </si>
+  <si>
+    <t>Arrival &amp; Registration</t>
+  </si>
+  <si>
+    <t>8:00-9:00</t>
+  </si>
+  <si>
+    <t>9:00-10:00</t>
+  </si>
+  <si>
+    <t>2:35-3:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,20 +192,6 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -200,7 +201,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -223,11 +224,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -238,10 +250,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,189 +570,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" customWidth="1"/>
-    <col min="8" max="8" width="19.5" customWidth="1"/>
-    <col min="9" max="10" width="26.1640625" customWidth="1"/>
-    <col min="11" max="11" width="20.1640625" customWidth="1"/>
-    <col min="12" max="12" width="28.5" customWidth="1"/>
-    <col min="13" max="13" width="31" customWidth="1"/>
+    <col min="1" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="10" max="11" width="26.1640625" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="28.5" customWidth="1"/>
+    <col min="14" max="14" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="109" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="83" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>40</v>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>31</v>
-      </c>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M8" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="109" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>42</v>
-      </c>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactor: update presenter names for sessions on ungrading and AI pedagogy
</commit_message>
<xml_diff>
--- a/session_schedule_by_slot.xlsx
+++ b/session_schedule_by_slot.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjohnson/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E93D415-0816-6E43-93E7-E3FD0127C7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D86975-7E20-7F4D-BE7C-AC3AC1D28585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15200" yWindow="800" windowWidth="14880" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="800" windowWidth="30000" windowHeight="18680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
   <si>
     <t>Time Slot</t>
   </si>
@@ -164,6 +165,9 @@
   </si>
   <si>
     <t>2:35-3:00</t>
+  </si>
+  <si>
+    <t>Conrau-Lewis: Overcoming students’ initial reactions to AI through text-based experiments</t>
   </si>
 </sst>
 </file>
@@ -573,7 +577,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -710,6 +714,9 @@
       <c r="L4" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="M4" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -736,7 +743,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>7</v>
@@ -781,7 +788,7 @@
         <v>25</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>21</v>
@@ -806,6 +813,160 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J11" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B227DA6F-A021-D34C-821E-58EDFCCCC061}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="169" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" ht="141" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="99" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="211" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="99" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="141" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="141" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="127" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="99" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="113" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="155" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="71" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix encoding issues in session descriptions and titles, update presenter details, and add new session on AI literacy through literature.
</commit_message>
<xml_diff>
--- a/session_schedule_by_slot.xlsx
+++ b/session_schedule_by_slot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjohnson/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D86975-7E20-7F4D-BE7C-AC3AC1D28585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0C7BE8-2985-DF4C-85CA-6B12160F8BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="800" windowWidth="30000" windowHeight="18680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3280" yWindow="640" windowWidth="34720" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>Time Slot</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Conrau-Lewis: Overcoming students’ initial reactions to AI through text-based experiments</t>
+  </si>
+  <si>
+    <t>Blue:  Do Androids Dream? Teaching AI Literacy Through Literature</t>
   </si>
 </sst>
 </file>
@@ -243,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -265,6 +268,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -796,6 +802,9 @@
       <c r="L6" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="M6" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="N6" s="3" t="s">
         <v>30</v>
       </c>

</xml_diff>